<commit_message>
Arreglo de bug a causa de los NaN
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaquin.deferrari\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e24deacd15ff203/Proyectos/Proyecto Sociogramas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F13A08-F793-4643-ADFE-83B5DF4BBB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{90F13A08-F793-4643-ADFE-83B5DF4BBB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{757951CD-01D8-4E4A-94D3-472143A20CEA}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="105" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -660,9 +660,6 @@
   </si>
   <si>
     <t>niña30</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1156,7 @@
   <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1175,7 @@
     <col min="16" max="16" width="11" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="14" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="16" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="0.28515625" customWidth="1"/>
+    <col min="19" max="19" width="2.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51.75" x14ac:dyDescent="0.25">
@@ -1867,9 +1864,6 @@
       <c r="U11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="W11" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="12" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -2104,9 +2098,7 @@
       <c r="N15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="13">
-        <v>0</v>
-      </c>
+      <c r="O15" s="13"/>
       <c r="P15" s="10">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>